<commit_message>
fixed the save error bug due to unchanged file name
</commit_message>
<xml_diff>
--- a/Templates/Data/Unames1.xlsx
+++ b/Templates/Data/Unames1.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="16" uniqueCount="2">
   <si>
     <t>Created by LibXL trial version 4.6.0. Please buy the LibXL full version for removing this message.</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV1"/>
+  <dimension ref="A1:IV11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -339,6 +342,61 @@
       <c r="IU1" s="1"/>
       <c r="IV1" s="1"/>
     </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:IV1"/>

</xml_diff>